<commit_message>
Feinspezifikation erweitert + UI
</commit_message>
<xml_diff>
--- a/_IPA/IPA_2019/Projektplanung.xlsx
+++ b/_IPA/IPA_2019/Projektplanung.xlsx
@@ -207,21 +207,21 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -526,7 +526,7 @@
   <dimension ref="A2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,235 +536,235 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>2</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>2</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>20</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>4</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>20</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>40</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>5</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>5</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>5</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>5</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>10</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9" t="s">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>8</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7" t="s">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>16</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>8</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="2">
         <f>SUM(C4:C24)</f>
         <v>156</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>